<commit_message>
finally added tokenization etc, forgot to do it before
</commit_message>
<xml_diff>
--- a/extracting_sentence_contexts/data_to_view/contexts_all_together/excel_ver/contexts_spectator.xlsx
+++ b/extracting_sentence_contexts/data_to_view/contexts_all_together/excel_ver/contexts_spectator.xlsx
@@ -205,13 +205,13 @@
     <t>factious</t>
   </si>
   <si>
-    <t>You have twice or thrice observed in your Discourse, that Hypocrisy is the very Foundation of our Education; and that an Ability to dissemble our affections, is a professed Part of our Breeding. These, and such other Reflections, are sprinkled up and down the Writings of all Ages, by Authors, who leave behind them Memorials of their Resentment against the Scorn of particular Women, in Invectives against the whole Sex. Such a Writer, I doubt not, was the celebrated Petronius, who invented the pleasant Aggravations of the Frailty of the Ephesian Lady; but when we consider this Question between the Sexes, which has been either a Point of Dispute or Raillery ever since there were Men and Women, let us take Facts from plain People, and from such as have not either Ambition or Capacity to embellish their Narrations with any Beauties of Imagination. I was the other Day amusing myself with Ligon's Account of Barbadoes; and, in Answer to your well-wrought Tale, I will give you (as it dwells upon my Memory) out of that honest Traveller, in his fifty fifth page, the History of Inkle and Yarico2. Mr.</t>
-  </si>
-  <si>
-    <t>A Cook should not live at the Boot, nor a Shoemaker at the roasted Pig; and yet, for want of this Regulation, I have seen a Goat set up before the Door of a Perfumer, and the French King's Head at a Sword-Cutler's. An ingenious Foreigner observes, that several of those Gentlemen who value themselves upon their Families, and overlook such as are bred to Trade, bear the Tools of their Fore-fathers in their Coats of Arms. I will not examine how true this is in Fact: But though it may not be necessary for Posterity thus to set up the Sign of their Fore-fathers; I think it highly proper for those who actually profess the Trade, to shew some such Marks of it before their Doors. When the Name gives an Occasion for an ingenious Sign-post, I would likewise advise the Owner to take that Opportunity of letting the World know who he is. It would have been ridiculous for the ingenious Mrs.</t>
-  </si>
-  <si>
-    <t>I must confess, the Design and Transactions of too many Clubs are trifling, and manifestly of no consequence to the Nation or Publick Weal: Those I'll give you up. But you must do me then the Justice to own, that nothing can be more useful or laudable than the Scheme we go upon. To avoid Nicknames and Witticisms, we call ourselves The Hebdomadal Meeting: Our President continues for a Year at least, and sometimes four or five: We are all Grave, Serious, Designing Men, in our Way: We think it our Duty, as far as in us lies, to take care the Constitution receives no Harm, — Ne quid detrimenti Res capiat publica — To censure Doctrines or Facts, Persons or Things, which we don't like; To settle the Nation at home, and to carry on the War abroad, where and in what manner we see fit: If other People are not of our Opinion, we can't help that. 'Twere better they were. Moreover, we now and then condescend to direct, in some measure, the little Affairs of our own University. Verily, Mr.</t>
+    <t>You have twice or thrice observed in your Discourse, that Hypocrisy is the very Foundation of our Education; and that an Ability to dissemble our affections, is a professed Part of our Breeding. These, and such other Reflections, are sprinkled up and down the Writings of all Ages, by Authors, who leave behind them Memorials of their Resentment against the Scorn of particular Women, in Invectives against the whole Sex. Such a Writer, I doubt not, was the celebrated Petronius, who invented the pleasant Aggravations of the Frailty of the Ephesian Lady; but when we consider this Question between the Sexes, which has been either a Point of Dispute or Raillery ever since there were Men and Women, let us take Facts from plain People, and from such as have not either Ambition or Capacity to embellish their Narrations with any Beauties of Imagination. I was the other Day amusing myself with Ligon's Account of Barbadoes; and, in Answer to your well-wrought Tale, I will give you (as it dwells upon my Memory) out of that honest Traveller, in his fifty fifth page, the History of Inkle and Yarico2. Mr. Thomas Inkle of London, aged twenty Years, embarked in the Downs, on the good Ship called the Achilles, bound for the West Indies, on the 16th of June 1647, in order to improve his Fortune by Trade and Merchandize.</t>
+  </si>
+  <si>
+    <t>A Cook should not live at the Boot, nor a Shoemaker at the roasted Pig; and yet, for want of this Regulation, I have seen a Goat set up before the Door of a Perfumer, and the French King's Head at a Sword-Cutler's. An ingenious Foreigner observes, that several of those Gentlemen who value themselves upon their Families, and overlook such as are bred to Trade, bear the Tools of their Fore-fathers in their Coats of Arms. I will not examine how true this is in Fact: But though it may not be necessary for Posterity thus to set up the Sign of their Fore-fathers; I think it highly proper for those who actually profess the Trade, to shew some such Marks of it before their Doors. When the Name gives an Occasion for an ingenious Sign-post, I would likewise advise the Owner to take that Opportunity of letting the World know who he is.</t>
+  </si>
+  <si>
+    <t>But you must do me then the Justice to own, that nothing can be more useful or laudable than the Scheme we go upon. To avoid Nicknames and Witticisms, we call ourselves The Hebdomadal Meeting: Our President continues for a Year at least, and sometimes four or five: We are all Grave, Serious, Designing Men, in our Way: We think it our Duty, as far as in us lies, to take care the Constitution receives no Harm, — Ne quid detrimenti Res capiat publica — To censure Doctrines or Facts, Persons or Things, which we don't like; To settle the Nation at home, and to carry on the War abroad, where and in what manner we see fit: If other People are not of our Opinion, we can't help that. 'Twere better they were. Moreover, we now and then condescend to direct, in some measure, the little Affairs of our own University.</t>
   </si>
   <si>
     <t>However, to avoid publick Blood-shed, as soon as his Passion is wrought to its Height, he follows his Sister the whole length of the Stage, and forbears killing her till they are both withdrawn behind the Scenes. I must confess, had he murder'd her before the Audience, the Indecency might have been greater; but as it is, it appears very unnatural, and looks like killing in cold Blood. To give my Opinion upon this Case; the Fact ought not to have been represented, but to have been told, if there was any Occasion for it. It may not be unacceptable to the Reader, to see how Sophocles has conducted a Tragedy under the like delicate Circumstances. Orestes was in the same Condition with Hamlet in Shakespear, his Mother having murdered his Father, and taken possession of his Kingdom in Conspiracy with her Adulterer.</t>
@@ -220,8 +220,7 @@
     <t>Our other Interpreter used to talk very much of a kind of Animal called a Tory, that was as great a Monster as the Whig, and would treat us as ill for being Foreigners. These two Creatures, it seems, are born with a secret Antipathy to one another, and engage when they meet as naturally as the Elephant and the Rhinoceros. But as we saw none of either of these Species, we are apt to think that our Guides deceived us with Misrepresentations and Fictions, and amused us with an Account of such Monsters as are not really in their Country. These Particulars we made a shift to pick out from the Discourse of our Interpreters; which we put together as well as we could, being able to understand but here and there a Word of what they said, and afterwards making up the Meaning of it among ourselves. The Men of the Country are very cunning and ingenious in handicraft Works; but withal so very idle, that we often saw young lusty raw-boned Fellows carried up and down the Streets in little covered Rooms by a Couple of Porters, who are hired for that Service.</t>
   </si>
   <si>
-    <t>I look upon these writers as Goths in Poetry, who, like those in Architecture, not being able to come up to the beautiful Simplicity of the old Greeks and Romans, have endeavoured to supply its place with all the Extravagancies of an irregular Fancy. Mr. Dryden makes a very handsome Observation, on Ovid's writing a Letter from Dido to Æneas, in the following Words6.
-    'Ovid' says he, (speaking of Virgil's Fiction of Dido and Æneas) 'takes it up after him, even in the same Age, and makes an Ancient Heroine of Virgil's new-created Dido; dictates a Letter for her just before her Death to the ungrateful Fugitive; and, very unluckily for himself, is for measuring a Sword with a Man so much superior in Force to him on the same Subject. I think I may be Judge of this, because I have translated both. The famous Author of the Art of Love has nothing of his own; he borrows all from a greater Master in his own Profession, and, which is worse, improves nothing which he finds: Nature fails him, and being forced to his old Shift, he has Recourse to Witticism.</t>
+    <t>I look upon these writers as Goths in Poetry, who, like those in Architecture, not being able to come up to the beautiful Simplicity of the old Greeks and Romans, have endeavoured to supply its place with all the Extravagancies of an irregular Fancy. Mr. Dryden makes a very handsome Observation, on Ovid's writing a Letter from Dido to Æneas, in the following Words6. 'Ovid' says he, (speaking of Virgil's Fiction of Dido and Æneas) 'takes it up after him, even in the same Age, and makes an Ancient Heroine of Virgil's new-created Dido; dictates a Letter for her just before her Death to the ungrateful Fugitive; and, very unluckily for himself, is for measuring a Sword with a Man so much superior in Force to him on the same Subject. I think I may be Judge of this, because I have translated both.</t>
   </si>
   <si>
     <t>But though the Language is mean, the Thoughts , as I have before said, from one end to the other are natural2, and therefore cannot fail to please those who are not Judges of Language, or those who, notwithstanding they are Judges of Language, have a true3 and unprejudiced Taste of Nature. The Condition, Speech, and Behaviour of the dying Parents, with the Age, Innocence, and Distress of the Children, are set forth in such tender Circumstances, that it is impossible for a Reader of common Humanity4 not to be affected with them. As for the Circumstance of the Robin-red-breast, it is indeed a little Poetical Ornament; and to shew the Genius of the Author5 amidst all his Simplicity, it is just the same kind of Fiction which one of the greatest of the Latin Poets has made use of upon a parallel Occasion; I mean that Passage in Horace, where he describes himself when he was a Child, fallen asleep in a desart Wood, and covered with Leaves by the Turtles that took pity on him. Me fabulosa Vulture in Apulo,
@@ -234,19 +233,17 @@
     <t>The Knight seeing his Habitation reduced to3 so small a Compass, and himself in a manner shut out of his own House, upon the Death of his Mother ordered all the Apartments4 to be flung open, and exorcised by his Chaplain, who lay in every Room one after another, and by that Means dissipated the Fears which had so long reigned in the Family. I should not have been thus particular upon these ridiculous Horrours, did I not find them so very much prevail in all Parts of the Country. At the same time I think a Person who is thus terrify'd with the Imagination of Ghosts and Spectres much more reasonable than one who, contrary to the Reports of all Historians sacred and prophane, ancient and modern, and to the Traditions of all Nations, thinks the Appearance of Spirits fabulous and groundless: Could not I give myself up to this general Testimony of Mankind, I should to the Relations of particular Persons who are now living, and whom I cannot distrust in other Matters of Fact. I might here add, that not only the Historians, to whom we may join the Poets, but likewise the Philosophers of Antiquity have favoured this Opinion. Lucretius himself, though by the Course of his Philosophy he was obliged to maintain that the Soul did not exist separate from the Body, makes no Doubt of the Reality of Apparitions, and that Men have often appeared after their Death.</t>
   </si>
   <si>
-    <t>I might here add, that not only the Historians, to whom we may join the Poets, but likewise the Philosophers of Antiquity have favoured this Opinion. Lucretius himself, though by the Course of his Philosophy he was obliged to maintain that the Soul did not exist separate from the Body, makes no Doubt of the Reality of Apparitions, and that Men have often appeared after their Death. This I think very remarkable; he was so pressed with the Matter of Fact which he could not have the Confidence to deny, that he was forced to account for it by one of the most absurd unphilosophical Notions that was ever started. He tells us, That the Surfaces of all Bodies are perpetually flying off from their respective Bodies, one after another; and that these Surfaces or thin Cases that included each other whilst they were joined in the Body like the Coats of an Onion, are sometimes seen entire when they are separated from it; by which means we often behold the Shapes and Shadows of Persons who are either dead or absent5. I shall dismiss this Paper with a Story out of Josephus, not so much for the sake of the Story it self as for the moral Reflections with which the Author concludes it, and which I shall here set down in his own Words.
-    'Glaphyra the Daughter of King Archelaus, after the Death of her two first Husbands (being married to a third, who was Brother to her first Husband, and so passionately in love with her that he turned off his former Wife to make room for this Marriage) had a very odd kind of Dream.</t>
-  </si>
-  <si>
-    <t>However, for the sake of our passed Loves, I shall free thee from thy present Reproach, and make thee mine for ever. Glaphyra told this Dream to several Women of her Acquaintance, and died soon after.6 I thought this Story might not be impertinent in this Place, wherein I speak of those Kings: Besides that, the Example deserves to be taken notice of as it contains a most certain Proof of the Immortality of the Soul, and of Divine Providence. If any Man thinks these Facts incredible, let him enjoy his own Opinion to himself, but let him not endeavour to disturb the Belief of others, who by Instances of this Nature are excited to the Study of Virtue.' 
-L.</t>
+    <t>I might here add, that not only the Historians, to whom we may join the Poets, but likewise the Philosophers of Antiquity have favoured this Opinion. Lucretius himself, though by the Course of his Philosophy he was obliged to maintain that the Soul did not exist separate from the Body, makes no Doubt of the Reality of Apparitions, and that Men have often appeared after their Death. This I think very remarkable; he was so pressed with the Matter of Fact which he could not have the Confidence to deny, that he was forced to account for it by one of the most absurd unphilosophical Notions that was ever started. He tells us, That the Surfaces of all Bodies are perpetually flying off from their respective Bodies, one after another; and that these Surfaces or thin Cases that included each other whilst they were joined in the Body like the Coats of an Onion, are sometimes seen entire when they are separated from it; by which means we often behold the Shapes and Shadows of Persons who are either dead or absent5. I shall dismiss this Paper with a Story out of Josephus, not so much for the sake of the Story it self as for the moral Reflections with which the Author concludes it, and which I shall here set down in his own Words.</t>
+  </si>
+  <si>
+    <t>However, for the sake of our passed Loves, I shall free thee from thy present Reproach, and make thee mine for ever. Glaphyra told this Dream to several Women of her Acquaintance, and died soon after.6 I thought this Story might not be impertinent in this Place, wherein I speak of those Kings: Besides that, the Example deserves to be taken notice of as it contains a most certain Proof of the Immortality of the Soul, and of Divine Providence. If any Man thinks these Facts incredible, let him enjoy his own Opinion to himself, but let him not endeavour to disturb the Belief of others, who by Instances of this Nature are excited to the Study of Virtue.' L.</t>
   </si>
   <si>
     <t>Tull.translation 
 We know the highest Pleasure our Minds are capable of enjoying with Composure, when we read Sublime Thoughts communicated to us by Men of great Genius and Eloquence. Such is the Entertainment we meet with in the Philosophick Parts of Cicero's Writings. Truth and good Sense have there so charming a Dress, that they could hardly be more agreeably represented with the Addition of Poetical Fiction and the Power of Numbers. This ancient Author, and a modern one, had fallen into my Hands within these few Days; and the Impressions they have left upon me, have at the present quite spoiled me for a merry Fellow. The Modern is that admirable Writer the Author of The Theory of the Earth.</t>
   </si>
   <si>
-    <t>The Truth of it is, if all the Happiness that is dispersed through the whole Race of Mankind in this World were drawn together, and put into the Possession of any single Man, it would not make a very happy Being. Though on the contrary, if the Miseries of the whole Species were fixed in a single Person, they would make a very miserable one. I am engaged in this Subject by the following Letter, which, though subscribed by a fictitious Name, I have reason to believe is not Imaginary. Mr. Spectator2, 'I am one of your Disciples, and endeavour to live up to your Rules, which I hope will incline you to pity my Condition: I shall open it to you in a very few Words.</t>
+    <t>The Truth of it is, if all the Happiness that is dispersed through the whole Race of Mankind in this World were drawn together, and put into the Possession of any single Man, it would not make a very happy Being. Though on the contrary, if the Miseries of the whole Species were fixed in a single Person, they would make a very miserable one. I am engaged in this Subject by the following Letter, which, though subscribed by a fictitious Name, I have reason to believe is not Imaginary. Mr. Spectator2, 'I am one of your Disciples, and endeavour to live up to your Rules, which I hope will incline you to pity my Condition: I shall open it to you in a very few Words. About three Years since a Gentleman, whom, I am sure, you yourself would have approved, made his Addresses to me.</t>
   </si>
   <si>
     <t>But, submitting these Matters to your more serious Consideration,
@@ -260,29 +257,21 @@
     <t>He then called together the most faithful of his Counsellors, and acquainting them with his Secretary's Crime, asked them their Advice in so delicate an Affair. They most of them gave their Opinion, that the Person could not be too severely punished who had thus dishonoured his Master. Upon the whole Debate, the Emperor declared it was his Opinion, that Eginhart's Punishment would rather encrease than diminish the Shame of his Family, and that therefore he thought it the most adviseable to wear out the Memory of the Fact, by marrying him to his Daughter. Accordingly Eginhart was called in, and acquainted by the Emperor, that he should no longer have any Pretence of complaining his Services were not rewarded, for that the Princess Imma should be given him7 in Marriage, with a Dower suitable to her Quality; which was soon after performed accordingly. L.</t>
   </si>
   <si>
-    <t>Thieves! and the Constable with his Attendants seized my expecting Lover. I kept my self unobserved till I saw the Crowd sufficiently encreased, and then appeared to declare the Goods to be mine; and had the Satisfaction to see my Man of Mode put into the Round-House, with the stolen Wares by him, to be produced in Evidence against him the next Morning. This Matter is notoriously known to be Fact; and I have been contented to save my Prentice, and take a Year's Rent of this mortified Lover, not to appear further in the Matter. This was some Penance; but, Sir, is this enough for a Villany of much more pernicious Consequence than the Trifles for which he was to have been indicted? Should not you, and all Men of any Parts or Honour, put things upon so right a Foot, as that such a Rascal should not laugh at the Imputation of what he was really guilty, and dread being accused of that for which he was arrested?</t>
+    <t>and the Constable with his Attendants seized my expecting Lover. I kept my self unobserved till I saw the Crowd sufficiently encreased, and then appeared to declare the Goods to be mine; and had the Satisfaction to see my Man of Mode put into the Round-House, with the stolen Wares by him, to be produced in Evidence against him the next Morning. This Matter is notoriously known to be Fact; and I have been contented to save my Prentice, and take a Year's Rent of this mortified Lover, not to appear further in the Matter. This was some Penance; but, Sir, is this enough for a Villany of much more pernicious Consequence than the Trifles for which he was to have been indicted? Should not you, and all Men of any Parts or Honour, put things upon so right a Foot, as that such a Rascal should not laugh at the Imputation of what he was really guilty, and dread being accused of that for which he was arrested?</t>
   </si>
   <si>
     <t>My Correspondents take the Hint I give them, and pursue it into Speculations which I never thought of at my first starting it. This has been the Fate of my Paper on the Match of Grinning, which has already produced a second Paper on parallel Subjects, and brought me the following Letter by the last Post. I shall not premise any thing to it further than that it is built on Matter of Fact, and is as follows. Sir,
-    'You have already obliged the World with a Discourse upon Grinning, and have since proceeded to Whistling, from whence you at length came1 to Yawning; from this, I think, you may make a very natural Transition to Sleeping. I therefore recommend to you for the Subject of a Paper the following Advertisement, which about two Months ago was given into every Body's Hands, and may be seen with some Additions in the Daily Courant of August the Ninth.
-        'Nicholas Hart2, who slept last Year in St.</t>
-  </si>
-  <si>
-    <t>Sir,
-    'You have already obliged the World with a Discourse upon Grinning, and have since proceeded to Whistling, from whence you at length came1 to Yawning; from this, I think, you may make a very natural Transition to Sleeping. I therefore recommend to you for the Subject of a Paper the following Advertisement, which about two Months ago was given into every Body's Hands, and may be seen with some Additions in the Daily Courant of August the Ninth.
-        'Nicholas Hart2, who slept last Year in St. Bartholomew's Hospital, intends to sleep this Year at the Cock and Bottle in Little-Britain.'
-    Having since inquired into the Matter of Fact, I find that the above-mentioned Nicholas Hart is every Year seized with a periodical Fit of Sleeping, which begins upon the Fifth of August, and ends on the Eleventh of the same Month: That
+    'You have already obliged the World with a Discourse upon Grinning, and have since proceeded to Whistling, from whence you at length came1 to Yawning; from this, I think, you may make a very natural Transition to Sleeping. I therefore recommend to you for the Subject of a Paper the following Advertisement, which about two Months ago was given into every Body's Hands, and may be seen with some Additions in the Daily Courant of August the Ninth.</t>
+  </si>
+  <si>
+    <t>I therefore recommend to you for the Subject of a Paper the following Advertisement, which about two Months ago was given into every Body's Hands, and may be seen with some Additions in the Daily Courant of August the Ninth. 'Nicholas Hart2, who slept last Year in St. Bartholomew's Hospital, intends to sleep this Year at the Cock and Bottle in Little-Britain.' Having since inquired into the Matter of Fact, I find that the above-mentioned Nicholas Hart is every Year seized with a periodical Fit of Sleeping, which begins upon the Fifth of August, and ends on the Eleventh of the same Month: That
         On the First of that Month he grew dull;
-        On the Second, appeared drowsy;
-        On the Third, fell a yawning;
+        On the Second, appeared drowsy; On the Third, fell a yawning;
         On the Fourth, began to nod;
         On the Fifth, dropped asleep;
         On the Sixth, was heard to snore;
-        On the Seventh, turned himself in his Bed;
-        On the Eighth, recovered his former Posture;
-        On the Ninth fell a stretching;
-        On the Tenth about Midnight, awaked;
-        On the Eleventh in the Morning called for a little Small-Beer. This Account I have extracted out of the Journal of this sleeping Worthy, as it has been faithfully kept by a Gentleman of Lincoln's-Inn, who has undertaken to be his Historiographer. I have sent it to you, not only as it represents the Actions of Nicholas Hart, but as it seems a very natural Picture of the Life of many an honest English Gentleman, whose whole History very often consists of Yawning, Nodding, Stretching, Turning, Sleeping, Drinking, and the like extraordinary Particulars.</t>
+        On the Seventh, turned himself in his Bed; On the Eighth, recovered his former Posture;
+        On the Ninth fell a stretching;</t>
   </si>
   <si>
     <t>The Levée of a great Man is laid after the same manner, and twenty Whispers, false Alarms, and private Intimations, pass backward and forward from the Porter, the Valet, and the Patron himself, before the gaping Crew who are to pay their Court are gathered together: When the Scene is ready, the Doors fly open and discover his Lordship. There are several Ways of making this first Appearance: you may be either half dressed, and washing your self, which is indeed the most stately; but this Way of Opening is peculiar to Military Men, in whom there is something graceful in exposing themselves naked; but the Politicians, or Civil Officers, have usually affected to be more reserved, and preserve a certain Chastity of Deportment. Whether it be Hieroglyphical or not, this Difference in the Military and Civil List, I will not say; but have3 ever understood the Fact to be, that the close Minister is buttoned up, and the brave Officer open-breasted on these Occasions. However that is, I humbly conceive the Business of a Levée is to receive the Acknowledgments of a Multitude, that a Man is Wise, Bounteous4, Valiant and Powerful. When the first Shot of Eyes is5 made, it is wonderful to observe how much Submission the Patron's Modesty can bear, and how much Servitude the Client's Spirit can descend to.</t>
@@ -293,7 +282,8 @@
   </si>
   <si>
     <t>I assure you without Flattery it has saved a Prentice of mine from Ruin; and in Token of Gratitude as well as for the Benefit of my Family, I have put it in a Frame and Glass, and hung it behind my Counter. I shall take Care to make my young ones read it every Morning, to fortify them against such pernicious Rascals. I know not whether what you writ was Matter of Fact, or your own Invention; but this I will take my Oath on, the first Part is so exactly like what happened to my Prentice, that had I read your Paper then, I should have taken your Method to have secured a Villain. Go on and prosper. Your most obliged Humble Servant,
-    Mr.</t>
+    Mr. Spectator,
+    'Without Raillery, I desire you to insert this Word for Word in your next, as you value a Lover's Prayers.</t>
   </si>
   <si>
     <t>For my part, I think there is no Reflection more astonishing, than to consider one of these Gentlemen spending a fair Fortune, running in every Body's Debt without the least Apprehension of a future Reckoning, and at last leaving not only his own Children, but possibly those of other People, by his Means, in starving Circumstances; while a Fellow, whom one would scarce suspect to have a humane Soul, shall perhaps raise a vast Estate out of Nothing, and be the Founder of a Family capable of being very considerable in their Country, and doing many illustrious Services to it. That this Observation is just, Experience has put beyond all Dispute. But though the Fact be so evident and glaring, yet the Causes of it are still in the Dark; which makes me persuade my self, that it would be no unacceptable Piece of Entertainment to the Town, to inquire into the hidden Sources of so unaccountable an Evil. I am,
@@ -302,13 +292,15 @@
   </si>
   <si>
     <t>Hor.1translation
-You very often hear People, after a Story has been told with some entertaining Circumstances, tell it over again with Particulars that destroy the Jest, but give Light into the Truth of the Narration. This sort of Veracity, though it is impertinent, has something amiable in it, because it proceeds from the Love of Truth, even in frivolous Occasions. If such honest Amendments do not promise an agreeable Companion, they do a sincere Friend; for which Reason one should allow them so much of our Time, if we fall into their Company, as to set us right in Matters that can do us no manner of Harm, whether the Facts be one Way or the other. Lies which are told out of Arrogance and Ostentation a Man should detect in his own Defence, because he should not be triumphed over; Lies which are told out of Malice he should expose, both for his own sake and that of the rest of Mankind, because every Man should rise against a common Enemy: But the officious Liar many have argued is to be excused, because it does some Man good, and no Man hurt. The Man who made more than ordinary speed from a Fight in which the Athenians were beaten, and told them they had obtained a complete Victory, and put the whole City into the utmost Joy and Exultation, was check'd by the Magistrates for his Falshood; but excused himself by saying, O Athenians! am I your Enemy because I gave you two happy Days?</t>
-  </si>
-  <si>
-    <t>The3 inexpressible Force wherewith he lays them on, sufficiently shows the Evidence and Strength of his Conviction. His Zeal for a good Author is indeed outrageous, and breaks down every Fence and Partition, every Board and Plank, that stands within the Expression of his Applause. As I do not care for terminating my Thoughts in barren Speculations, or in Reports of pure Matter of Fact, without drawing something from them for the Advantage of my Countrymen, I shall take the Liberty to make an humble Proposal, that whenever the Trunk-maker shall depart this Life, or whenever he shall have lost the Spring of his Arm by Sickness, old Age, Infirmity, or the like, some able-bodied Critick should be advanced to this Post, and have a competent Salary settled on him for Life, to be furnished with Bamboos for Operas, Crabtree-Cudgels for Comedies, and Oaken Plants for Tragedy, at the publick Expence. And to the End that this Place should be always disposed of according to Merit, I would have none preferred to it, who has not given convincing Proofs both of a sound Judgment and a strong Arm, and who could not, upon Occasion, either knock down an Ox, or write a Comment upon Horace's Art of Poetry. In short, I would have him a due Composition of Hercules and Apollo, and so rightly qualified for this important Office, that the Trunk-maker may not be missed by our Posterity.</t>
-  </si>
-  <si>
-    <t>The poor Woman upon this Faints away in a Fit, recovers, and is now run distracted. As she had no Design to defraud her Husband, but was willing only to participate in his good Fortune, every one pities her, but thinks her Husband's Punishment but just. This, Sir, is Matter of Fact, and would, if the Persons and Circumstances were greater, in a well-wrought Play be called Beautiful Distress. I have only sketched it out with Chalk, and know a good Hand can make a moving Picture with worse Materials. Sir, &amp;c.</t>
+You very often hear People, after a Story has been told with some entertaining Circumstances, tell it over again with Particulars that destroy the Jest, but give Light into the Truth of the Narration. This sort of Veracity, though it is impertinent, has something amiable in it, because it proceeds from the Love of Truth, even in frivolous Occasions. If such honest Amendments do not promise an agreeable Companion, they do a sincere Friend; for which Reason one should allow them so much of our Time, if we fall into their Company, as to set us right in Matters that can do us no manner of Harm, whether the Facts be one Way or the other. Lies which are told out of Arrogance and Ostentation a Man should detect in his own Defence, because he should not be triumphed over; Lies which are told out of Malice he should expose, both for his own sake and that of the rest of Mankind, because every Man should rise against a common Enemy: But the officious Liar many have argued is to be excused, because it does some Man good, and no Man hurt. The Man who made more than ordinary speed from a Fight in which the Athenians were beaten, and told them they had obtained a complete Victory, and put the whole City into the utmost Joy and Exultation, was check'd by the Magistrates for his Falshood; but excused himself by saying, O Athenians!</t>
+  </si>
+  <si>
+    <t>His Zeal for a good Author is indeed outrageous, and breaks down every Fence and Partition, every Board and Plank, that stands within the Expression of his Applause. As I do not care for terminating my Thoughts in barren Speculations, or in Reports of pure Matter of Fact, without drawing something from them for the Advantage of my Countrymen, I shall take the Liberty to make an humble Proposal, that whenever the Trunk-maker shall depart this Life, or whenever he shall have lost the Spring of his Arm by Sickness, old Age, Infirmity, or the like, some able-bodied Critick should be advanced to this Post, and have a competent Salary settled on him for Life, to be furnished with Bamboos for Operas, Crabtree-Cudgels for Comedies, and Oaken Plants for Tragedy, at the publick Expence. And to the End that this Place should be always disposed of according to Merit, I would have none preferred to it, who has not given convincing Proofs both of a sound Judgment and a strong Arm, and who could not, upon Occasion, either knock down an Ox, or write a Comment upon Horace's Art of Poetry. In short, I would have him a due Composition of Hercules and Apollo, and so rightly qualified for this important Office, that the Trunk-maker may not be missed by our Posterity.</t>
+  </si>
+  <si>
+    <t>The poor Woman upon this Faints away in a Fit, recovers, and is now run distracted. As she had no Design to defraud her Husband, but was willing only to participate in his good Fortune, every one pities her, but thinks her Husband's Punishment but just. This, Sir, is Matter of Fact, and would, if the Persons and Circumstances were greater, in a well-wrought Play be called Beautiful Distress. I have only sketched it out with Chalk, and know a good Hand can make a moving Picture with worse Materials. Sir, &amp;c.
+    Mr. Spectator,
+    I am what the World calls a warm Fellow, and by good Success in Trade I have raised myself to a Capacity of making some Figure in the World; but no matter for that.</t>
   </si>
   <si>
     <t>We see Man and Woman in the highest Innocence and Perfection, and in the most abject State of Guilt and Infirmity. The two last Characters are, indeed, very common and obvious, but the two first are not only more magnificent, but more new5 than any Characters either in Virgil or Homer, or indeed in the whole Circle of Nature. Milton was so sensible of this Defect in the Subject of his Poem, and of the few Characters it would afford him, that he has brought into it two Actors of a Shadowy and Fictitious Nature, in the Persons of Sin and Death6, by which means he has wrought into7 the Body of his Fable a very beautiful and well-invented Allegory. But notwithstanding the Fineness of this Allegory may attone for it in some measure; I cannot think that Persons of such a Chymerical Existence are proper Actors in an Epic Poem; because there is not that measure of Probability annexed to them, which is requisite in Writings of this kind, as I shall shew more at large hereafter. Virgil has, indeed, admitted Fame as an Actress in the Æneid, but the Part she acts is very short, and none of the most admired Circumstances in that Divine Work.</t>
@@ -320,7 +312,7 @@
     <t>But this is not all; an honest private Man often grows cruel and abandoned, when converted into an absolute Prince. Give a Man Power of doing what he pleases with Impunity, you extinguish his Fear, and consequently overturn in him one of the great Pillars of Morality. This too we find confirmed by Matter of Fact. How many hopeful Heirs apparent to grand Empires, when in the Possession of them, have become such Monsters of Lust and Cruelty as are a Reproach to Human Nature. Some tell us we ought to make our Governments on Earth like that in Heaven, which, say they, is altogether Monarchical and Unlimited.</t>
   </si>
   <si>
-    <t>If we look into the Sentiments, I think they are sometimes defective under the following Heads: First, as there are several of them too much pointed, and some that degenerate even into Punns. Of this last kind I am afraid is that in the First Book, where speaking of the Pigmies, he calls them,
+    <t>First, as there are several of them too much pointed, and some that degenerate even into Punns. Of this last kind I am afraid is that in the First Book, where speaking of the Pigmies, he calls them,
     —The small Infantry
     Warrdon by Cranes—
 Another Blemish that13 appears in some of his Thoughts, is his frequent Allusion to Heathen Fables, which are not certainly of a Piece with the Divine Subject, of which he treats. I do not find fault with these Allusions, where the Poet himself represents them as fabulous, as he does in some Places, but where he mentions them as Truths and Matters of Fact. The Limits of my Paper will not give me leave to be particular in Instances of this kind; the Reader will easily remark them in his Perusal of the Poem. A third fault in his Sentiments, is an unnecessary Ostentation of Learning, which likewise occurs very frequently.</t>
@@ -345,7 +337,7 @@
     <t>The ninth Book, which we are here to consider, is raised upon that brief Account in Scripture, wherein we are told that the Serpent was more subtle than any Beast of the Field, that he tempted the Woman to eat of the forbidden Fruit, that she was overcome by this Temptation, and that Adam followed her Example. From these few Particulars, Milton has formed one of the most Entertaining Fables that Invention ever produced. He has disposed of these several Circumstances among so many beautiful and natural Fictions of his own, that his whole Story looks only like a Comment upon sacred Writ, or rather seems to be a full and compleat Relation of what the other is only an Epitome. I have insisted the longer on this Consideration, as I look upon the Disposition and Contrivance of the Fable to be the principal Beauty of the ninth Book, which has more Story in it, and is fuller of Incidents, than any other in the whole Poem. Satan's traversing the Globe, and still keeping within the Shadow of the Night, as fearing to be discovered by the Angel of the Sun, who had before detected him, is one of those beautiful Imaginations with which he introduces this his second Series of Adventures.</t>
   </si>
   <si>
-    <t>If his Reproaches are true, if thou art the envious ill-natur'd Man he takes thee for, give thy self another Turn, become mild, affable and obliging, and his Reproaches of thee naturally cease: His Reproaches may indeed continue, but thou art no longer the Person whom he reproaches. I often apply this Rule to my self; and when I hear of a Satyrical Speech or Writing that is aimed at me, I examine my own Heart, whether I deserve it or not. If I bring in a Verdict against my self, I endeavour to rectify my Conduct for the future in those particulars which have drawn the Censure upon me; but if the whole Invective be grounded upon a Falsehood, I trouble my self no further about it, and look upon my Name at the Head of it to signify no more than one of those fictitious Names made use of by an Author to introduce an imaginary Character. Why should a Man be sensible of the Sting of a Reproach, who is a Stranger to the Guilt that is implied in it? or subject himself to the Penalty, when he knows he has never committed the Crime? This is a Piece of Fortitude, which every one owes to his own Innocence, and without which it is impossible for a Man of any Merit or Figure to live at Peace with himself in a Country that abounds with Wit and Liberty.</t>
+    <t>If his Reproaches are true, if thou art the envious ill-natur'd Man he takes thee for, give thy self another Turn, become mild, affable and obliging, and his Reproaches of thee naturally cease: His Reproaches may indeed continue, but thou art no longer the Person whom he reproaches. I often apply this Rule to my self; and when I hear of a Satyrical Speech or Writing that is aimed at me, I examine my own Heart, whether I deserve it or not. If I bring in a Verdict against my self, I endeavour to rectify my Conduct for the future in those particulars which have drawn the Censure upon me; but if the whole Invective be grounded upon a Falsehood, I trouble my self no further about it, and look upon my Name at the Head of it to signify no more than one of those fictitious Names made use of by an Author to introduce an imaginary Character. Why should a Man be sensible of the Sting of a Reproach, who is a Stranger to the Guilt that is implied in it? or subject himself to the Penalty, when he knows he has never committed the Crime?</t>
   </si>
   <si>
     <t>The Watchman was so affected with it, that he bought her, and has taken her in Partner, only altering their Hours of Duty from Night to Day. The Town has come into it, and they live very comfortably. This is the Matter of Fact: Now I desire you, who are a profound Philosopher, to consider this Alliance of Instinct and Reason; your Speculation may turn very naturally upon the Force the superior Part of Mankind may have upon the Spirits of such as, like this Watchman, may be very near the Standard of Geese. And you may add to this practical Observation, how in all Ages and Times the World has been carry'd away by odd unaccountable things, which one would think would pass upon no Creature which had Reason; and, under the Symbol of this Goose, you may enter into the Manner and Method of leading Creatures, with their Eyes open, thro' thick and thin, for they know not what, they know not why. All which is humbly submitted to your Spectatorial Wisdom by,
@@ -379,7 +371,7 @@
     Hor. As the Writers in Poetry and Fiction borrow their several Materials from outward Objects, and join them together at their own Pleasure, there are others who are obliged to follow Nature more closely, and to take entire Scenes out of her. Such are Historians, natural Philosophers, Travellers, Geographers, and in a Word, all who describe visible Objects of a real Existence. It is the most agreeable Talent of an Historian, to be able to draw up his Armies and fight his Battels in proper Expressions, to set before our Eyes the Divisions, Cabals, and Jealousies of great Men, and to lead us Step by Step into the several Actions and Events of his History.</t>
   </si>
   <si>
-    <t>Disagreeable Passions pleasing when raised by apt Descriptions. Why Terror and Grief are pleasing to the Mind when excited by Descriptions. A particular Advantage the Writers in Poetry and Fiction have to please the Imagination. What Liberties are allowed them. Paper IX 	Of that kind of Poetry which Mr.</t>
+    <t>Disagreeable Passions pleasing when raised by apt Descriptions. Why Terror and Grief are pleasing to the Mind when excited by Descriptions. A particular Advantage the Writers in Poetry and Fiction have to please the Imagination. What Liberties are allowed them. Paper IX 	Of that kind of Poetry which Mr. Dryden calls the Fairy Way of Writing.</t>
   </si>
   <si>
     <t>Who the Best among the English. Of Emblematical Persons. Paper X 	What Authors please the Imagination who have nothing to do with Fiction. How History pleases the Imagination. How the Authors of the new Philosophy please the Imagination.</t>
@@ -388,7 +380,7 @@
     <t>The Reader's Curiosity is raised and satisfied every Moment, and his Passions disappointed or gratified, without being detained in a State of uncertainty from Day to Day, or lying at the Mercy of Sea and1 Wind. In short, the Mind is not here kept in a perpetual Gape after Knowledge, nor punished with that Eternal Thirst, which is the Portion of all our modern News-mongers and Coffee-house Politicians. All Matters of Fact, which a Man did not know before, are News to him; and I do not see how any Haberdasher in Cheapside is more concerned in the present Quarrel of the Cantons, than he was in that of the League. At least, I believe every one will allow me, it is of more Importance to an Englishman to know the History of his Ancestors, than that of his Contemporaries who live upon the Banks of the Danube or the Borysthenes. As for those who are of another Mind, I shall recommend to them the following Letter, from a Projector, who is willing to turn a Penny by this remarkable Curiosity of his Countrymen.</t>
   </si>
   <si>
-    <t>As for those who are of another Mind, I shall recommend to them the following Letter, from a Projector, who is willing to turn a Penny by this remarkable Curiosity of his Countrymen. Mr. SPECTATOR,
+    <t>At least, I believe every one will allow me, it is of more Importance to an Englishman to know the History of his Ancestors, than that of his Contemporaries who live upon the Banks of the Danube or the Borysthenes. As for those who are of another Mind, I shall recommend to them the following Letter, from a Projector, who is willing to turn a Penny by this remarkable Curiosity of his Countrymen. Mr. SPECTATOR,
     'You must have observed, that Men who frequent Coffee-houses, and delight in News, are pleased with every thing that is Matter of Fact, so it be what they have not heard before. A Victory, or a Defeat, are equally agreeable to them. The shutting of a Cardinal's Mouth pleases them one Post, and the opening of it another.</t>
   </si>
   <si>
@@ -398,9 +390,12 @@
     <t>Well, it came at last to the Sermon, and our young Lady would not lose her Part in that neither; for she fixed her Eye upon the Preacher, and as he said any thing she approved, with one of Charles Mathers's fine Tablets she set down the Sentence, at once shewing her fine Hand, the Gold-Pen, her Readiness in Writing, and her Judgment in chusing what to write. To sum up what I intend by this long and particular Account, I mean to appeal to you, whether it is reasonable that such a Creature as this shall come from a jaunty Part of the Town, and give herself such violent Airs, to the disturbance of an innocent and inoffensive Congregation, with her Sublimities. The Fact, I assure you, was as I have related; but I had like to have forgot another very considerable Particular. As soon as Church was done, she immediately stepp'd out of her Pew, and fell into the finest pitty-pat Air, forsooth, wonderfully out of Countenance, tossing her Head up and down as she swam along the Body of the Church. I, with several others of the Inhabitants, follow'd her out, and saw her hold up her Fan to an Hackney-Coach at a Distance, who immediately came up to her, and she whipp'd into it with great Nimbleness, pull'd the Door with a bowing Mein, as if she had been used to a better Glass.</t>
   </si>
   <si>
-    <t>Arb.translation
+    <t>No. 521
+Tuesday, October 28, 1712
+Steele
+    Vera redit facies, dissimulata perit. P. Arb.translation
     Mr. SPECTATOR,
-    I have been for many Years loud in this Assertion, That there are very few that can see or hear, I mean that can report what they have seen or heard; and this thro' Incapacity or Prejudice, one of which disables almost every Man who talks to you from representing things as he ought. For which Reason I am come to a Resolution of believing nothing I hear; and I contemn the Men given to Narration under the Appellation of a Matter of Fact Man: And according to me, a Matter of Fact Man is one whose Life and Conversation is spent in the Report of what is not Matter of Fact. I remember when Prince Eugene was here, there was no knowing his Height or Figure, till you, Mr. SPECTATOR, gave the Publick Satisfaction in that Matter.</t>
+    I have been for many Years loud in this Assertion, That there are very few that can see or hear, I mean that can report what they have seen or heard; and this thro' Incapacity or Prejudice, one of which disables almost every Man who talks to you from representing things as he ought. For which Reason I am come to a Resolution of believing nothing I hear; and I contemn the Men given to Narration under the Appellation of a Matter of Fact Man: And according to me, a Matter of Fact Man is one whose Life and Conversation is spent in the Report of what is not Matter of Fact. I remember when Prince Eugene was here, there was no knowing his Height or Figure, till you, Mr. SPECTATOR, gave the Publick Satisfaction in that Matter. In Relations, the Force of the Expression lies very often more in the Look, the Tone of Voice, or the Gesture, than the Words themselves; which being repeated in any other Manner by the Undiscerning, bear a very different Interpretation from their original Meaning.</t>
   </si>
   <si>
     <t>I have had the Honour to travel with this Gentleman I speak of in Search of one of his Falshoods; and have been present when they have described the very Man they have spoken to, as him who first reported it, tall or short, black or fair, a Gentleman or a Raggamuffin, according as they liked the Intelligence. I have heard one of our ingenious Writers of News say, that when he has had a Customer come with an Advertisement of an Apprentice or a Wife run away, he has deSir ed the Advertiser to compose himself a little, before he dictated the Description of the Offender: For when a Person is put into a publick Paper by a Man who is angry with him, the real Description of such Person is hid in the Deformity with which the angry Man described him; therefore this Fellow always made his Customers describe him as he would the Day before he offended, or else he was sure he would never find him out. These and many other Hints I could suggest to you for the Elucidation of all Fictions; but I leave it to your own Sagacity to improve or neglect this Speculation. I am, Sir ,
@@ -420,62 +415,41 @@
     <t>Secondly, because I would extort a little Praise from such who will never applaud any thing whose Author is known and certain. Thirdly, because it gave me an Opportunity of introducing a great variety of Characters into my Work, which could not have been done, had I always written in the Person of the Spectator. Fourthly, because the Dignity Spectatorial would have suffered, had I published as from my self those several ludicrous Compositions which I have ascribed to fictitious Names and Characters. And lastly, because they often serve to bring in, more naturally, such additional Reflections as have been placed at the End of them. There are others who have likewise done me a very particular Honour, though undesignedly.</t>
   </si>
   <si>
-    <t>No Nation in the World delights so much in having their own, or Friends, or Relations Pictures; whether from their National Good-Nature, or having a love to Painting, and not being encouraged in the great Article of Religious Pictures, which the Purity of our Worship refuses the free use of, or from whatever other Cause. Our Helps are not inferior to those of any other People, but rather they are greater; for what the Antique Statues and Bas-reliefs which Italy enjoys are to the History-Painters, the Beautiful and noble Faces with which England is confessed to abound, are to Face-Painters; and besides we have the greatest number of the Works of the best Masters in that kind of any People, not without a competent number of those of the most excellent in every other part of Painting. And for Encouragement, the Wealth and Generosity of the English Nation affords that in such a degree, as Artists have no reason to complain.
-    'And accordingly in Fact, Face-Painting is no where so well performed as in England: I know not whether it has lain in your way to observe it, but I have, and pretend to be a tolerable Judge. I have seen what is done abroad, and can assure you, that the Honour of that Branch of Painting is justly due to us. I appeal to the judicious Observers for the Truth of what I assert.</t>
+    <t>Our Helps are not inferior to those of any other People, but rather they are greater; for what the Antique Statues and Bas-reliefs which Italy enjoys are to the History-Painters, the Beautiful and noble Faces with which England is confessed to abound, are to Face-Painters; and besides we have the greatest number of the Works of the best Masters in that kind of any People, not without a competent number of those of the most excellent in every other part of Painting. And for Encouragement, the Wealth and Generosity of the English Nation affords that in such a degree, as Artists have no reason to complain. 'And accordingly in Fact, Face-Painting is no where so well performed as in England: I know not whether it has lain in your way to observe it, but I have, and pretend to be a tolerable Judge. I have seen what is done abroad, and can assure you, that the Honour of that Branch of Painting is justly due to us. I appeal to the judicious Observers for the Truth of what I assert.</t>
   </si>
   <si>
     <t>It is much more difficult to converse with the World in a real than a personated Character. That might pass for Humour in the Spectator, which would look like Arrogance in a Writer who sets his Name to his Work. The Fictitious Person might contemn those who disapproved him, and extoll his own Performances, without giving Offence. He might assume a mock-Authority, without being looked upon as vain and conceited. The Praises or Censures of himself fall only upon the Creature of his Imaginations; and if any one finds fault with him, the Author may reply with the Philosopher of old, Thou dost but beat the Case of Anaxarchus.</t>
   </si>
   <si>
-    <t>Every insignificant Author fancies it of Importance to the World, to know that he writ his Book in the Country, that he did it to pass away some of his idle Hours, that it was published at the Importunity of Friends, or that his natural Temper, Studies or Conversations, directed him to the Choice of his Subject.
-    —Id populus curat scilicet. Such Informations cannot but be highly improving to the Reader. In Works of Humour, especially when a Man writes under a fictitious Personage, the talking of one's self may give some Diversion to the Publick; but I would advise every other Writer never to speak of himself, unless there be something very considerable in his Character: Tho' I am sensible this Rule will be of little Use in the World, because there is no Man who fancies his Thoughts worth publishing, that does not look upon himself as a considerable Person. I shall close this Paper with a Remark upon such as are Egotists in Conversation: These are generally the vain or shallow part of Mankind, People being naturally full of themselves when they have nothing else in them. There is one kind of Egotists which is very common in the World, tho' I do not remember that any Writer has taken Notice of them; I mean those empty conceited Fellows, who repeat as Sayings of their own, or some of their particular Friends, several Jests which were made before they were born, and which every one who has conversed in the World has heard a hundred times over.</t>
+    <t>—Id populus curat scilicet. Such Informations cannot but be highly improving to the Reader. In Works of Humour, especially when a Man writes under a fictitious Personage, the talking of one's self may give some Diversion to the Publick; but I would advise every other Writer never to speak of himself, unless there be something very considerable in his Character: Tho' I am sensible this Rule will be of little Use in the World, because there is no Man who fancies his Thoughts worth publishing, that does not look upon himself as a considerable Person. I shall close this Paper with a Remark upon such as are Egotists in Conversation: These are generally the vain or shallow part of Mankind, People being naturally full of themselves when they have nothing else in them. There is one kind of Egotists which is very common in the World, tho' I do not remember that any Writer has taken Notice of them; I mean those empty conceited Fellows, who repeat as Sayings of their own, or some of their particular Friends, several Jests which were made before they were born, and which every one who has conversed in the World has heard a hundred times over.</t>
   </si>
   <si>
     <t>Sir
-    'I was the other Day reading the Life of Mahomet. Among many other Extravagancies, I find it recorded of that Impostor, that in the fourth Year of his Age the Angel Gabriel caught him up, while he was among his Play-fellows, and, carrying him aside, cut open his Breast, plucked out his Heart, and wrung out of it that black Drop of Blood, in which, say the Turkish Divines, is contained the Fomes Peccati, so that he was free from Sin ever after. I immediately said to my self, tho' this Story be a Fiction, a very good Moral may be drawn from it, would every Man but apply it to himself, and endeavour to squeeze out of his Heart whatever Sins or ill Qualities he finds in it.
-    'While my Mind was wholly taken up with this Contemplation, I insensibly fell into a most pleasing Slumber, when methought two Porters entered my Chamber, carrying a large Chest between them. After having set it down in the middle of the Room they departed. I immediately endeavour'd to open what was sent me, when a Shape, like that in which we paint our Angels, appeared before me, and forbad me.</t>
+    'I was the other Day reading the Life of Mahomet. Among many other Extravagancies, I find it recorded of that Impostor, that in the fourth Year of his Age the Angel Gabriel caught him up, while he was among his Play-fellows, and, carrying him aside, cut open his Breast, plucked out his Heart, and wrung out of it that black Drop of Blood, in which, say the Turkish Divines, is contained the Fomes Peccati, so that he was free from Sin ever after. I immediately said to my self, tho' this Story be a Fiction, a very good Moral may be drawn from it, would every Man but apply it to himself, and endeavour to squeeze out of his Heart whatever Sins or ill Qualities he finds in it. 'While my Mind was wholly taken up with this Contemplation, I insensibly fell into a most pleasing Slumber, when methought two Porters entered my Chamber, carrying a large Chest between them. After having set it down in the middle of the Room they departed.</t>
   </si>
   <si>
     <t>Is the Force of Self-Love abated, or its Interest prejudiced by Benevolence? So far from it, that Benevolence, though a distinct Principle, is extreamly serviceable to Self-Love, and then doth most Service when 'tis least designed. But to descend from Reason to Matter of Fact; the Pity which arises on Sight of Persons in Distress, and the Satisfaction of Mind which is the Consequence of having removed them into a happier State, are instead of a thousand Arguments to prove such a thing as a disinterested Benevolence. Did Pity proceed from a Reflection we make upon our Liableness to the same ill Accidents we see befall others, it were nothing to the present Purpose; but this is assigning an artificial Cause of a natural Passion, and can by no Means be admitted as a tolerable Account of it, because Children and Persons most Thoughtless about their own Condition, and incapable of entering into the Prospects of Futurity, feel the most violent Touches of Compassion. And then as to that charming Delight which immediately follows the giving Joy to another, or relieving his Sorrow, and is, when the Objects are numerous, and the kindness of Importance really inexpressible, what can this be owing to but a Consciousness of a Man's having done some thing Praise-worthy, and expressive of a great Soul?</t>
   </si>
   <si>
-    <t>He deSir es in his Postscript to know, whether, from a constant Success in them, he may not promise himself to succeed in her Esteem at last. Another who is very prolix in his Narrative writes me Word, that having sent a Venture beyond Sea, he took Occasion one Night to fancy himself gone along with it, and grown on a sudden the richest Man in all the Indies. Having been there about a Year or two, a Gust of Wind that forced open his Casement blew him over to his native Country again, where awaking at Six a Clock, and the Change of the Air not agreeing with him, he turned to his Left Side in order to a second Voyage: but e'er he could get on Shipboard, was unfortunately apprehended for stealing a Horse, try'd and condemn'd for the Fact, and in a fair way of being executed, if some Body stepping hastily into his Chamber had not brought him a Reprieve. This Fellow too wants Mr. Shadow's Advice, who, I dare say, would bid him be content to rise after his first Nap, and learn to be satisfied as soon as Nature is.</t>
-  </si>
-  <si>
-    <t>The Clouds invelop'd Heav'n from Human Sight,
-        Quench'd every Star, and put out ev'ry Light;
-        Now Real Thunder grumbles in the Skies,
-        And in disdainful Murmurs Rome defies;
-        Nor doth its answer'd Challenge Rome decline;
-        But whilst both Parties in full Consort join,
-        While Heav'n and Earth in Rival Peals resound,
-        The doubtful Cracks the Hearer's Sense confound;
-        Whether the Claps of Thunderbolts they hear,
-        Or else the Burst of Canon wounds their Ear;
-        Whether Clouds raged by struggling Metals rent,
-        Or struggling Clouds in Roman Metals pent. But O, my Muse, the whole Adventure tell,
-        As ev'ry Accident in order fell. Tall Groves of Trees the Hadrian Tow'r surround,
+    <t>He deSir es in his Postscript to know, whether, from a constant Success in them, he may not promise himself to succeed in her Esteem at last. Another who is very prolix in his Narrative writes me Word, that having sent a Venture beyond Sea, he took Occasion one Night to fancy himself gone along with it, and grown on a sudden the richest Man in all the Indies. Having been there about a Year or two, a Gust of Wind that forced open his Casement blew him over to his native Country again, where awaking at Six a Clock, and the Change of the Air not agreeing with him, he turned to his Left Side in order to a second Voyage: but e'er he could get on Shipboard, was unfortunately apprehended for stealing a Horse, try'd and condemn'd for the Fact, and in a fair way of being executed, if some Body stepping hastily into his Chamber had not brought him a Reprieve. This Fellow too wants Mr. Shadow's Advice, who, I dare say, would bid him be content to rise after his first Nap, and learn to be satisfied as soon as Nature is. The next is a publick-spirited Gentleman, who tells me, That on the Second of September at Night the whole City was on Fire, and would certainly have been reduced to Ashes again by this Time, if he had not flown over it with the New River on his Back, and happily extinguished the Flames before they had prevailed too far.</t>
+  </si>
+  <si>
+    <t>But O, my Muse, the whole Adventure tell, As ev'ry Accident in order fell. Tall Groves of Trees the Hadrian Tow'r surround,
         Fictitious Trees with Paper Garlands crown'd,
         These know no Spring, but when their Bodies sprout
-        In Fire, and shoot their gilded Blossoms out;
-        When blazing Leaves appear above their Head,
+        In Fire, and shoot their gilded Blossoms out; When blazing Leaves appear above their Head,
         And into branching Flames their Bodies spread. Whilst real Thunder splits the Firmament,
         And Heav'n's whole Roof in one vast Cleft is rent,
         The three-fork'd Tongue amidst the Rupture lolls,
-        Then drops and on the Airy Turret falls. The Trees now kindle, and the Garland burns,
-        And thousand Thunderbolts for one returns.</t>
-  </si>
-  <si>
-    <t>Corneille was merciful, and in the fifth act bred in his Menteur a new fancy for Lucrece, so that the marriage at cross purposes was rather agreeable to him. Steele, in adapting the Menteur as his Lying Lover, altered the close in sharp accordance with that 'just regard to a reforming age,' which caused him (adapting a line in his 'Procession' then unprinted) to write in his Prologue to it, 'Pleasure must still have something that's severe.' Having translated Corneille's translations of Garcia and Tristan (Dorante and Cliton) into Young Bookwit and Latine, he transformed the servant into a college friend, mumming as servant because, since 'a prating servant is necessary in intrigues,' the two had 'cast lots who should be the other's footman for the present expedition.' Then he adapted the French couplets into pleasant prose comedy, giving with a light touch the romancing of feats of war and of an entertainment on the river, but at last he turned desperately serious, and sent his Young Bookwit to Newgate on a charge of killing the gentleman — here called Lovemore — who was at last to win the hand of the lady whom the Liar loved. In his last act, opening in Newgate, Steele started with blank verse, and although Lovemore of course was not dead, and Young Bookwit got at last more than a shadow of a promise the other lady in reward for his repentance, the changes in construction of the play took it beyond the bounds of comedy, and were, in fact, excellent morality but not good art. And this is what Steele means when he says that he had his play damned for its piety. With that strong regard for the drama which cannot well be wanting to the man who has an artist's vivid sense of life, Steele never withdrew his good will from the players, never neglected to praise a good play, and, I may add, took every fair occasion of suggesting to the town the subtlety of Shakespeare's genius.</t>
-  </si>
-  <si>
-    <t>I know no party; but the truth of the question is what I will support as well as I can, when any man I honour is attacked.'
-John Forster, whose keen insight into the essentials of literature led him to write an essay upon each of the two great founders of the latest period of English literature, Defoe and Steele, has pointed out in his masterly essay upon Steele that Swift denies having spoken of Steele as bridled by his friend, and does so in a way that frankly admits Steele's right to be jealous of the imputation. Mr. Forster justly adds that throughout Swift's intimate speech to Stella,
-    'whether his humours be sarcastic or polite, the friendship of Steele and Addison is for ever suggesting some annoyance to himself, some mortification, some regret, but never once the doubt that it was not intimate and sincere, or that into it entered anything inconsistent with a perfect equality.'
-Six months after Addison's death Steele wrote (in No. 12 of the Theatre, and I am again quoting facts cited by John Forster),
-    'that there never was a more strict friendship than between himself and Addison, nor had they ever any difference but what proceeded from their different way of pursuing the same thing; the one waited and stemmed the torrent, while the other too often plunged into it; but though they thus had lived for some years past, shunning each other, they still preserved the most passionate concern for their mutual welfare; and when they met they were as unreserved as boys, and talked of the greatest affairs, upon which they saw where they differed, without pressing (what they knew impossible) to convert each other.' 
-As to the substance or worth of what thus divided them, Steele only adds the significant expression of his hope that, if his family is the worse, his country may be the better, 'for the mortification he has undergone.'
-Such, then, was the Friendship of which the Spectator is the abiding Monument. The Spectator was a modified continuation of the Tatler, and the Tatler was suggested by a portion of Defoe's Review. The Spectator belongs to the first days of a period when the people at large extended their reading power into departments of knowledge formerly unsought by them, and their favour was found generally to be more desirable than that of the most princely patron.</t>
+        Then drops and on the Airy Turret falls.</t>
+  </si>
+  <si>
+    <t>Having translated Corneille's translations of Garcia and Tristan (Dorante and Cliton) into Young Bookwit and Latine, he transformed the servant into a college friend, mumming as servant because, since 'a prating servant is necessary in intrigues,' the two had 'cast lots who should be the other's footman for the present expedition.' Then he adapted the French couplets into pleasant prose comedy, giving with a light touch the romancing of feats of war and of an entertainment on the river, but at last he turned desperately serious, and sent his Young Bookwit to Newgate on a charge of killing the gentleman — here called Lovemore — who was at last to win the hand of the lady whom the Liar loved. In his last act, opening in Newgate, Steele started with blank verse, and although Lovemore of course was not dead, and Young Bookwit got at last more than a shadow of a promise the other lady in reward for his repentance, the changes in construction of the play took it beyond the bounds of comedy, and were, in fact, excellent morality but not good art. And this is what Steele means when he says that he had his play damned for its piety. With that strong regard for the drama which cannot well be wanting to the man who has an artist's vivid sense of life, Steele never withdrew his good will from the players, never neglected to praise a good play, and, I may add, took every fair occasion of suggesting to the town the subtlety of Shakespeare's genius.</t>
+  </si>
+  <si>
+    <t>John Forster, whose keen insight into the essentials of literature led him to write an essay upon each of the two great founders of the latest period of English literature, Defoe and Steele, has pointed out in his masterly essay upon Steele that Swift denies having spoken of Steele as bridled by his friend, and does so in a way that frankly admits Steele's right to be jealous of the imputation. Mr. Forster justly adds that throughout Swift's intimate speech to Stella,
+    'whether his humours be sarcastic or polite, the friendship of Steele and Addison is for ever suggesting some annoyance to himself, some mortification, some regret, but never once the doubt that it was not intimate and sincere, or that into it entered anything inconsistent with a perfect equality.' Six months after Addison's death Steele wrote (in No. 12 of the Theatre, and I am again quoting facts cited by John Forster),
+    'that there never was a more strict friendship than between himself and Addison, nor had they ever any difference but what proceeded from their different way of pursuing the same thing; the one waited and stemmed the torrent, while the other too often plunged into it; but though they thus had lived for some years past, shunning each other, they still preserved the most passionate concern for their mutual welfare; and when they met they were as unreserved as boys, and talked of the greatest affairs, upon which they saw where they differed, without pressing (what they knew impossible) to convert each other.' As to the substance or worth of what thus divided them, Steele only adds the significant expression of his hope that, if his family is the worse, his country may be the better, 'for the mortification he has undergone.'</t>
   </si>
   <si>
     <t>Steele gave only two lines to it:

</xml_diff>